<commit_message>
update utils and result
</commit_message>
<xml_diff>
--- a/utils/result.xlsx
+++ b/utils/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clarencewang/Desktop/SpringSem2019/ComputerArchitecture/Experiment/experiment/CRC/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE04E93-6229-344E-966B-356664EC3538}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E618D8D9-15F7-F040-A702-8A37F89FD5EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{6BFFEE9F-5270-4741-99BE-F7D46D831158}"/>
+    <workbookView xWindow="15120" yWindow="580" windowWidth="28040" windowHeight="17040" xr2:uid="{6BFFEE9F-5270-4741-99BE-F7D46D831158}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>LRU</t>
   </si>
@@ -385,15 +385,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86AF70AC-657B-2244-93C2-2037CCC8E81B}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -403,8 +403,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>400</v>
       </c>
@@ -414,8 +417,11 @@
       <c r="C2">
         <v>44.405999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>11.305999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>401</v>
       </c>
@@ -425,8 +431,11 @@
       <c r="C3">
         <v>61.677999999999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>88.179000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>403</v>
       </c>
@@ -436,8 +445,11 @@
       <c r="C4">
         <v>45.64</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>98.787999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>410</v>
       </c>
@@ -447,8 +459,11 @@
       <c r="C5">
         <v>99.662999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>88.962000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>416</v>
       </c>
@@ -458,8 +473,11 @@
       <c r="C6">
         <v>27.655000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>82.284999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>429</v>
       </c>
@@ -469,8 +487,11 @@
       <c r="C7">
         <v>76.683000000000007</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>111.264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>433</v>
       </c>
@@ -480,8 +501,11 @@
       <c r="C8">
         <v>76.948999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>95.216999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>434</v>
       </c>
@@ -491,8 +515,11 @@
       <c r="C9">
         <v>82.64</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>86.534999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>435</v>
       </c>
@@ -502,8 +529,11 @@
       <c r="C10">
         <v>74.372</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>91.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>436</v>
       </c>
@@ -513,8 +543,11 @@
       <c r="C11">
         <v>73.781999999999996</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>93.781999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>437</v>
       </c>
@@ -524,8 +557,11 @@
       <c r="C12">
         <v>81.12</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>89.251999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>444</v>
       </c>
@@ -535,8 +571,11 @@
       <c r="C13">
         <v>66.311999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>75.444999999999993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>445</v>
       </c>
@@ -546,8 +585,11 @@
       <c r="C14">
         <v>20.484000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>86.007000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>447</v>
       </c>
@@ -557,8 +599,11 @@
       <c r="C15">
         <v>41.786000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>100.492</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>450</v>
       </c>
@@ -568,8 +613,11 @@
       <c r="C16">
         <v>17.553999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>56.247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>453</v>
       </c>
@@ -579,8 +627,11 @@
       <c r="C17">
         <v>40.201999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>102.956</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>454</v>
       </c>
@@ -590,8 +641,11 @@
       <c r="C18">
         <v>38.319000000000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>96.728999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>456</v>
       </c>
@@ -601,8 +655,11 @@
       <c r="C19">
         <v>71.474000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>92.484999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>458</v>
       </c>
@@ -612,8 +669,11 @@
       <c r="C20">
         <v>94.103999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>97.311000000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>459</v>
       </c>
@@ -623,8 +683,11 @@
       <c r="C21">
         <v>84.153000000000006</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>89.581000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>462</v>
       </c>
@@ -634,8 +697,11 @@
       <c r="C22">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>90.14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>464</v>
       </c>
@@ -645,8 +711,11 @@
       <c r="C23">
         <v>71.772000000000006</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>86.165000000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>465</v>
       </c>
@@ -656,8 +725,11 @@
       <c r="C24">
         <v>79.430999999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>80.817999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>470</v>
       </c>
@@ -667,8 +739,11 @@
       <c r="C25">
         <v>99.938999999999993</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>98.933000000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>471</v>
       </c>
@@ -678,8 +753,11 @@
       <c r="C26">
         <v>60.055999999999997</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>91.725999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>473</v>
       </c>
@@ -689,8 +767,11 @@
       <c r="C27">
         <v>5.8470000000000004</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>96.027000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>482</v>
       </c>
@@ -700,8 +781,11 @@
       <c r="C28">
         <v>97.262</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>89.194000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>483</v>
       </c>
@@ -711,8 +795,11 @@
       <c r="C29">
         <v>67.58</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>94.662999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>999</v>
       </c>
@@ -721,6 +808,9 @@
       </c>
       <c r="C30">
         <v>96.320999999999998</v>
+      </c>
+      <c r="J30">
+        <v>52.363999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>